<commit_message>
[MS-WSSREST]: Update RS according to lastest version TD
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WSSREST/MS-WSSREST_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WSSREST/MS-WSSREST_RequirementSpecification.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$125</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="277">
   <si>
     <t>Req ID</t>
   </si>
@@ -377,9 +377,6 @@
     <t>MS-WSSREST_R110</t>
   </si>
   <si>
-    <t>MS-WSSREST_R111</t>
-  </si>
-  <si>
     <t>MS-WSSREST_R2</t>
   </si>
   <si>
@@ -692,9 +689,6 @@
     <t>MS-WSSREST_R112</t>
   </si>
   <si>
-    <t>MS-WSSREST_R113</t>
-  </si>
-  <si>
     <t>2.1</t>
   </si>
   <si>
@@ -743,12 +737,6 @@
     <t>[In Transport] No new transports are required except for those specified in [MS-ODATA] section 2.1.</t>
   </si>
   <si>
-    <t>[In Transport] It [MS-WSSREST] transmits these messages using the HTTP protocol as described in [RFC2616].</t>
-  </si>
-  <si>
-    <t>[In Transport] It [MS-WSSREST] transmits these messages [SHOULD]using the HTTPS protocol as described in [RFC2818].</t>
-  </si>
-  <si>
     <t>[In Common Message Syntax] This section contains common definitions that are used by this protocol.</t>
   </si>
   <si>
@@ -767,18 +755,6 @@
     <t>[In Elements] XML schema element definitions that are specific to a particular operation are described with the operation.</t>
   </si>
   <si>
-    <t>[In Elements] The List element is a container within a site (2) that stores list items.</t>
-  </si>
-  <si>
-    <t>[In Elements] The List item element is an individual entry within a list (1).</t>
-  </si>
-  <si>
-    <t>[In List] Each list (1) is represented as an EntitySet as specified in [MC-CSDL] section 2.1.17, which[EntitySet] contains Entities of a single EntityType as specified in [MC-CSDL] section 2.1.2.</t>
-  </si>
-  <si>
-    <t>[In List] This EntityType [for list] contains properties for every non-hidden field (2) in the list (1) whose field type is supported as well as a subset of hidden fields (2).</t>
-  </si>
-  <si>
     <t>[In List] List of supported field types and their mappings to the Entity Data Model property types is specified in section 2.2.2.2.</t>
   </si>
   <si>
@@ -791,21 +767,9 @@
     <t>[In List] The Field internal name: FileDirRef maps to the Entity Data Model property name: Path.</t>
   </si>
   <si>
-    <t>[In List] The owshiddenversion field (2) serves as the ETag property of the EntityType.</t>
-  </si>
-  <si>
-    <t>[In List] The FileDirRef field (2) represents the list item’s server-relative path.</t>
-  </si>
-  <si>
     <t>[In List Item] Every list item is represented as an Entity of a particular EntityType as specified in [MC-CSDL] section 2.1.2.</t>
   </si>
   <si>
-    <t>[In List Item] EntityTypes are created based on the list (1) to which the list item belongs.</t>
-  </si>
-  <si>
-    <t>[In List Item] Properties on the EntityType correspond to fields (2) of the list (1), with the field (2)’s type determining the type of the property, where these primitive and navigation property types are specified in [MC-CSDL] section 1.</t>
-  </si>
-  <si>
     <t>[In List Item] The following table details the mapping between field types, as specified in [MS-WSSTS] section 2.3.1, and Entity Data Model property types.</t>
   </si>
   <si>
@@ -950,12 +914,6 @@
     <t>[In Message Processing Events and Sequencing Rules] The element Attachment supports for delete operation.</t>
   </si>
   <si>
-    <t>[In Message Processing Events and Sequencing Rules] The element Choice supports for operations on choice field.</t>
-  </si>
-  <si>
-    <t>[In Message Processing Events and Sequencing Rules] The element multi-choice supports for operations on multi-choice fields.</t>
-  </si>
-  <si>
     <t>[In Message Processing Events and Sequencing Rules] The element Document supports for inserting a new document into a document library.</t>
   </si>
   <si>
@@ -975,9 +933,6 @@
   </si>
   <si>
     <t>[In Attachment] To facilitate delete operation support for list item attachments, an additional EntitySet is created.</t>
-  </si>
-  <si>
-    <t>[In Attachment] This EntitySet [support for list item attachment] does not correspond to any list (1).</t>
   </si>
   <si>
     <t>[In Attachment] Attachments are represented as a multi-valued navigation property on an Entity.</t>
@@ -1006,21 +961,6 @@
   </si>
   <si>
     <t>[In Attachment] For more details, see [MS-ODATA] section 3.2.5.</t>
-  </si>
-  <si>
-    <t>[In Choice or Multi-Choice Field] An EntitySet is created for every choice [or multi-choice] field (2) belonging to a list (1).</t>
-  </si>
-  <si>
-    <t>[In Choice or Multi-Choice Field] An EntitySet is created for [every choice or] multi-choice field (2) belonging to a list (1).</t>
-  </si>
-  <si>
-    <t>[In Choice or Multi-Choice Field] For a particular choice [or multi-choice field (2)], this EntitySet will contain Entities representing each option of the field (2) specified in the field definition of the field (2).</t>
-  </si>
-  <si>
-    <t>[In Choice or Multi-Choice Field] For a particular [choice or] multi-choice field (2), this EntitySet will contain Entities representing each option of the field (2) specified in the field definition of the field (2).</t>
-  </si>
-  <si>
-    <t>[In Choice or Multi-Choice Field] The EntityType for this EntitySet [of choice] as specified in [MC-CSDL] section 2.1.17 contains a single property "Value", which also serves as its [EntitySet's] EntityKey as specified in [MC-CSDL] section 2.1.5.</t>
   </si>
   <si>
     <t>[In Choice or Multi-Choice Field] The EntityType for this EntitySet [of multi-choice] as specified in [MC-CSDL] section 2.1.17 contains a single property "Value", which also serves as its [EntitySet's] EntityKey as specified in [MC-CSDL] section 2.1.5.</t>
@@ -1078,9 +1018,6 @@
     <t>[In Appendix C: Product Behavior] Implement does support the Field type: CrossProjectLink mapping to the Entity Data Model property type: Primitive (Boolean).(Microsoft SharePoint Foundation 2010 and Microsoft SharePointServer2010 follow this behavior )</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implement does support transmitting these messages using the HTTPS protocol as described in [RFC2818]. (Microsoft SharePoint Foundation 2010 and above products follow this behavior.)</t>
-  </si>
-  <si>
     <t>MS-WSSREST_R65:c</t>
   </si>
   <si>
@@ -1090,12 +1027,6 @@
     <t>MS-WSSREST_R29:i, MS-WSSREST_R102:i</t>
   </si>
   <si>
-    <t>MS-WSSREST_R111:i, MS-WSSREST_R102:i</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-WSSREST_R113.</t>
-  </si>
-  <si>
     <t>Verified by derived requirement: MS-WSSREST_R112.</t>
   </si>
   <si>
@@ -1109,12 +1040,63 @@
   </si>
   <si>
     <t>Open Specification Date:</t>
+  </si>
+  <si>
+    <t>[In Transport] Protocol server transmits request and response messages using the HTTP protocol as specified in [RFC2616] or the HTTPS protocol as specified in [RFC2818].</t>
+  </si>
+  <si>
+    <t>[In Elements] The List element is a container within a site that stores list items.</t>
+  </si>
+  <si>
+    <t>[In Elements] The List item element is an individual entry within a list.</t>
+  </si>
+  <si>
+    <t>[In List Item] EntityTypes are created based on the list to which the list item belongs.</t>
+  </si>
+  <si>
+    <t>[In Attachment] This EntitySet [support for list item attachment] does not correspond to any list.</t>
+  </si>
+  <si>
+    <t>[In List] Each list is represented as an EntitySet as specified in [MC-CSDL] section 2.1.18, which[EntitySet] contains Entities of a single EntityType as specified in [MC-CSDL] section 2.1.2.</t>
+  </si>
+  <si>
+    <t>[In List] This EntityType [for list] contains properties for every non-hidden field in the list whose field type is supported as well as a subset of hidden fields (2).</t>
+  </si>
+  <si>
+    <t>[In List] The FileDirRef field represents the list item’s server-relative path.</t>
+  </si>
+  <si>
+    <t>[In List Item] Properties on the EntityType correspond to fields (2) of the list, with the field’s type determining the type of the property, where these primitive and navigation property types are specified in [MC-CSDL] section 1.</t>
+  </si>
+  <si>
+    <t>[In Choice or Multi-Choice Field] An EntitySet is created for every choice [or multi-choice] field belonging to a list.</t>
+  </si>
+  <si>
+    <t>[In Choice or Multi-Choice Field] An EntitySet is created for [every choice or] multi-choice field belonging to a list.</t>
+  </si>
+  <si>
+    <t>[In Choice or Multi-Choice Field] For a particular choice [or multi-choice field], this EntitySet will contain Entities representing each option of the field specified in the field definition of the field.</t>
+  </si>
+  <si>
+    <t>[In Choice or Multi-Choice Field] For a particular [choice or] multi-choice field, this EntitySet will contain Entities representing each option of the field specified in the field definition of the field.</t>
+  </si>
+  <si>
+    <t>[In List] The owshiddenversion field serves as the ETag property, as specified in [MS-ODATA] section 2.2.5.4, of the EntityType.</t>
+  </si>
+  <si>
+    <t>[In Message Processing Events and Sequencing Rules] The element Choice supports for retrieve operations on choice field.</t>
+  </si>
+  <si>
+    <t>[In Message Processing Events and Sequencing Rules] The element multi-choice supports for retrieve operations on multi-choice fields.</t>
+  </si>
+  <si>
+    <t>[In Choice or Multi-Choice Field] The EntityType for this EntitySet [of choice] as specified in [MC-CSDL] section 2.1.18 contains a single property "Value", which also serves as its [EntitySet's] EntityKey as specified in [MC-CSDL] section 2.1.5.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -1380,21 +1362,6 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1418,6 +1385,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1935,8 +1917,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I127" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I127"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I125" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I125"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -2058,6 +2040,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2093,6 +2092,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2270,28 +2286,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2301,7 +2317,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2315,138 +2331,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="29">
-        <v>2.1</v>
+        <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="F3" s="12">
-        <v>41481</v>
+        <v>42566</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -2459,12 +2475,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -2477,12 +2493,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -2495,12 +2511,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -2513,60 +2529,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -2602,13 +2618,13 @@
     </row>
     <row r="20" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A20" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>165</v>
+        <v>148</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>260</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22" t="s">
@@ -2618,22 +2634,22 @@
         <v>3</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="21" spans="1:12" s="23" customFormat="1">
       <c r="A21" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>166</v>
+        <v>148</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>163</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
@@ -2643,22 +2659,22 @@
         <v>3</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="22" spans="1:12" s="23" customFormat="1">
       <c r="A22" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
@@ -2668,24 +2684,22 @@
         <v>3</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>277</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I22" s="24"/>
     </row>
     <row r="23" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
@@ -2702,15 +2716,15 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="24" spans="1:12" s="23" customFormat="1">
       <c r="A24" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="s">
@@ -2727,15 +2741,15 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="25" spans="1:12" s="23" customFormat="1">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -2752,22 +2766,22 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A26" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G26" s="22" t="s">
         <v>16</v>
@@ -2782,17 +2796,17 @@
         <v>49</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22" t="s">
         <v>19</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>16</v>
@@ -2802,28 +2816,28 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="28" spans="1:12" s="23" customFormat="1">
       <c r="A28" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>173</v>
+        <v>261</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
         <v>19</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I28" s="24"/>
     </row>
@@ -2832,10 +2846,10 @@
         <v>51</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>174</v>
+        <v>262</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
@@ -2852,15 +2866,15 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1">
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A30" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -2877,15 +2891,15 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A31" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>176</v>
+        <v>266</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
@@ -2907,10 +2921,10 @@
         <v>54</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -2920,47 +2934,47 @@
         <v>6</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H32" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="1:9" ht="30">
+      <c r="A33" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="24"/>
-    </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="30">
-      <c r="A33" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="24"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="34" spans="1:9" ht="30">
       <c r="A34" s="30" t="s">
         <v>56</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30" t="s">
@@ -2970,22 +2984,22 @@
         <v>6</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" ht="30">
+    <row r="35" spans="1:9">
       <c r="A35" s="30" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="30" t="s">
@@ -3007,10 +3021,10 @@
         <v>58</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="C36" s="32" t="s">
-        <v>181</v>
+        <v>152</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>273</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="30" t="s">
@@ -3032,10 +3046,10 @@
         <v>59</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>182</v>
+        <v>267</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30" t="s">
@@ -3052,15 +3066,15 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30" t="s">
@@ -3070,22 +3084,22 @@
         <v>6</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="30">
+    <row r="39" spans="1:9">
       <c r="A39" s="30" t="s">
         <v>61</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>184</v>
+        <v>263</v>
       </c>
       <c r="D39" s="30"/>
       <c r="E39" s="30" t="s">
@@ -3102,15 +3116,15 @@
       </c>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" ht="45">
       <c r="A40" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>185</v>
+        <v>268</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="30" t="s">
@@ -3120,22 +3134,22 @@
         <v>6</v>
       </c>
       <c r="G40" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" ht="45">
+    <row r="41" spans="1:9" ht="30">
       <c r="A41" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="30" t="s">
@@ -3152,15 +3166,15 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="30">
+    <row r="42" spans="1:9">
       <c r="A42" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30" t="s">
@@ -3170,22 +3184,22 @@
         <v>6</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" ht="30">
+    <row r="43" spans="1:9">
       <c r="A43" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="30" t="s">
@@ -3202,15 +3216,15 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" ht="30">
+    <row r="44" spans="1:9">
       <c r="A44" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30" t="s">
@@ -3227,15 +3241,15 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="30">
+    <row r="45" spans="1:9">
       <c r="A45" s="30" t="s">
         <v>67</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="30" t="s">
@@ -3252,15 +3266,15 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9">
       <c r="A46" s="30" t="s">
         <v>68</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30" t="s">
@@ -3277,15 +3291,15 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="30">
+    <row r="47" spans="1:9">
       <c r="A47" s="30" t="s">
         <v>69</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30" t="s">
@@ -3307,10 +3321,10 @@
         <v>70</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30" t="s">
@@ -3323,19 +3337,21 @@
         <v>15</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I48" s="32"/>
-    </row>
-    <row r="49" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="30" t="s">
         <v>71</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30" t="s">
@@ -3348,21 +3364,19 @@
         <v>15</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I49" s="32" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="30">
+        <v>21</v>
+      </c>
+      <c r="I49" s="32"/>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="30" t="s">
         <v>72</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30" t="s">
@@ -3379,15 +3393,15 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9">
       <c r="A51" s="30" t="s">
         <v>73</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="30" t="s">
@@ -3404,15 +3418,15 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9">
       <c r="A52" s="30" t="s">
         <v>74</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30" t="s">
@@ -3429,15 +3443,15 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9">
       <c r="A53" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="D53" s="30"/>
       <c r="E53" s="30" t="s">
@@ -3454,15 +3468,15 @@
       </c>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" ht="30">
+    <row r="54" spans="1:9">
       <c r="A54" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="30" t="s">
@@ -3479,15 +3493,15 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="30">
+    <row r="55" spans="1:9">
       <c r="A55" s="30" t="s">
         <v>77</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="D55" s="30"/>
       <c r="E55" s="30" t="s">
@@ -3504,15 +3518,15 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9">
       <c r="A56" s="30" t="s">
         <v>78</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="30" t="s">
@@ -3525,19 +3539,19 @@
         <v>15</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" ht="30">
+    <row r="57" spans="1:9">
       <c r="A57" s="30" t="s">
         <v>79</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="D57" s="30"/>
       <c r="E57" s="30" t="s">
@@ -3554,15 +3568,15 @@
       </c>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" ht="30">
+    <row r="58" spans="1:9">
       <c r="A58" s="30" t="s">
         <v>80</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30" t="s">
@@ -3579,15 +3593,15 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" ht="30">
+    <row r="59" spans="1:9">
       <c r="A59" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30" t="s">
@@ -3604,15 +3618,15 @@
       </c>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="30">
+    <row r="60" spans="1:9">
       <c r="A60" s="30" t="s">
         <v>82</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
@@ -3629,15 +3643,15 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9">
       <c r="A61" s="30" t="s">
         <v>83</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="s">
@@ -3654,15 +3668,15 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="30">
+    <row r="62" spans="1:9">
       <c r="A62" s="30" t="s">
         <v>84</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30" t="s">
@@ -3679,15 +3693,15 @@
       </c>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9">
       <c r="A63" s="30" t="s">
         <v>85</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30" t="s">
@@ -3704,15 +3718,15 @@
       </c>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" ht="30">
+    <row r="64" spans="1:9">
       <c r="A64" s="30" t="s">
         <v>86</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30" t="s">
@@ -3725,19 +3739,19 @@
         <v>15</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="30">
+    <row r="65" spans="1:9">
       <c r="A65" s="30" t="s">
         <v>87</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="30" t="s">
@@ -3754,15 +3768,15 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" s="30" t="s">
         <v>88</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30" t="s">
@@ -3784,10 +3798,10 @@
         <v>89</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30" t="s">
@@ -3804,40 +3818,40 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9">
       <c r="A68" s="30" t="s">
         <v>90</v>
       </c>
       <c r="B68" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F68" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G68" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H68" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9">
       <c r="A69" s="30" t="s">
         <v>91</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D69" s="30"/>
       <c r="E69" s="30" t="s">
@@ -3854,15 +3868,15 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9">
       <c r="A70" s="30" t="s">
         <v>92</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30" t="s">
@@ -3879,15 +3893,15 @@
       </c>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9">
       <c r="A71" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30" t="s">
@@ -3904,15 +3918,15 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="30" t="s">
         <v>94</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30" t="s">
@@ -3934,17 +3948,17 @@
         <v>95</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="D73" s="30"/>
       <c r="E73" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F73" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G73" s="30" t="s">
         <v>16</v>
@@ -3954,15 +3968,15 @@
       </c>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" ht="45">
+    <row r="74" spans="1:9" ht="30">
       <c r="A74" s="30" t="s">
         <v>96</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30" t="s">
@@ -3984,10 +3998,10 @@
         <v>97</v>
       </c>
       <c r="B75" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="D75" s="30"/>
       <c r="E75" s="30" t="s">
@@ -4009,17 +4023,17 @@
         <v>98</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F76" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G76" s="30" t="s">
         <v>16</v>
@@ -4029,22 +4043,22 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" ht="45">
+    <row r="77" spans="1:9" ht="30">
       <c r="A77" s="30" t="s">
         <v>99</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="D77" s="30"/>
       <c r="E77" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F77" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G77" s="30" t="s">
         <v>16</v>
@@ -4054,15 +4068,15 @@
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" ht="30">
+    <row r="78" spans="1:9">
       <c r="A78" s="30" t="s">
         <v>100</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30" t="s">
@@ -4072,10 +4086,10 @@
         <v>6</v>
       </c>
       <c r="G78" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H78" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I78" s="32"/>
     </row>
@@ -4084,10 +4098,10 @@
         <v>101</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="D79" s="30"/>
       <c r="E79" s="30" t="s">
@@ -4109,10 +4123,10 @@
         <v>102</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30" t="s">
@@ -4134,10 +4148,10 @@
         <v>103</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C81" s="32" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30" t="s">
@@ -4159,10 +4173,10 @@
         <v>104</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30" t="s">
@@ -4179,15 +4193,15 @@
       </c>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" ht="30">
+    <row r="83" spans="1:9" ht="45">
       <c r="A83" s="30" t="s">
         <v>105</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D83" s="30"/>
       <c r="E83" s="30" t="s">
@@ -4204,15 +4218,15 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="60">
+    <row r="84" spans="1:9" ht="30">
       <c r="A84" s="30" t="s">
         <v>106</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D84" s="30"/>
       <c r="E84" s="30" t="s">
@@ -4225,7 +4239,7 @@
         <v>15</v>
       </c>
       <c r="H84" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I84" s="32"/>
     </row>
@@ -4234,12 +4248,14 @@
         <v>107</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C85" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="D85" s="30"/>
+        <v>219</v>
+      </c>
+      <c r="D85" s="30" t="s">
+        <v>252</v>
+      </c>
       <c r="E85" s="30" t="s">
         <v>19</v>
       </c>
@@ -4259,13 +4275,13 @@
         <v>108</v>
       </c>
       <c r="B86" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C86" s="32" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D86" s="30" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="E86" s="30" t="s">
         <v>19</v>
@@ -4286,13 +4302,13 @@
         <v>109</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C87" s="32" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D87" s="30" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="E87" s="30" t="s">
         <v>19</v>
@@ -4304,7 +4320,7 @@
         <v>15</v>
       </c>
       <c r="H87" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I87" s="32"/>
     </row>
@@ -4313,13 +4329,13 @@
         <v>110</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C88" s="32" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D88" s="30" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="E88" s="30" t="s">
         <v>19</v>
@@ -4331,7 +4347,7 @@
         <v>15</v>
       </c>
       <c r="H88" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I88" s="32"/>
     </row>
@@ -4340,14 +4356,12 @@
         <v>111</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C89" s="32" t="s">
-        <v>234</v>
-      </c>
-      <c r="D89" s="30" t="s">
-        <v>273</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="D89" s="30"/>
       <c r="E89" s="30" t="s">
         <v>19</v>
       </c>
@@ -4367,10 +4381,10 @@
         <v>112</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C90" s="32" t="s">
-        <v>235</v>
+        <v>160</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>275</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30" t="s">
@@ -4383,7 +4397,7 @@
         <v>15</v>
       </c>
       <c r="H90" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I90" s="32"/>
     </row>
@@ -4392,10 +4406,10 @@
         <v>113</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="D91" s="30"/>
       <c r="E91" s="30" t="s">
@@ -4408,7 +4422,7 @@
         <v>15</v>
       </c>
       <c r="H91" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I91" s="32"/>
     </row>
@@ -4417,10 +4431,10 @@
         <v>114</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30" t="s">
@@ -4430,10 +4444,10 @@
         <v>6</v>
       </c>
       <c r="G92" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H92" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I92" s="32"/>
     </row>
@@ -4442,10 +4456,10 @@
         <v>115</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="D93" s="30"/>
       <c r="E93" s="30" t="s">
@@ -4455,10 +4469,10 @@
         <v>6</v>
       </c>
       <c r="G93" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H93" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I93" s="32"/>
     </row>
@@ -4470,9 +4484,11 @@
         <v>31</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="D94" s="30"/>
+        <v>226</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>253</v>
+      </c>
       <c r="E94" s="30" t="s">
         <v>19</v>
       </c>
@@ -4495,10 +4511,10 @@
         <v>31</v>
       </c>
       <c r="C95" s="32" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D95" s="30" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="E95" s="30" t="s">
         <v>19</v>
@@ -4522,10 +4538,10 @@
         <v>31</v>
       </c>
       <c r="C96" s="32" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="E96" s="30" t="s">
         <v>19</v>
@@ -4537,7 +4553,7 @@
         <v>15</v>
       </c>
       <c r="H96" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I96" s="32"/>
     </row>
@@ -4549,10 +4565,10 @@
         <v>31</v>
       </c>
       <c r="C97" s="32" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D97" s="30" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="E97" s="30" t="s">
         <v>19</v>
@@ -4564,11 +4580,11 @@
         <v>15</v>
       </c>
       <c r="H97" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I97" s="32"/>
     </row>
-    <row r="98" spans="1:9" ht="30">
+    <row r="98" spans="1:9">
       <c r="A98" s="30" t="s">
         <v>120</v>
       </c>
@@ -4576,11 +4592,9 @@
         <v>31</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="D98" s="30" t="s">
-        <v>274</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="D98" s="30"/>
       <c r="E98" s="30" t="s">
         <v>19</v>
       </c>
@@ -4588,14 +4602,14 @@
         <v>6</v>
       </c>
       <c r="G98" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H98" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I98" s="32"/>
     </row>
-    <row r="99" spans="1:9" ht="30">
+    <row r="99" spans="1:9">
       <c r="A99" s="30" t="s">
         <v>121</v>
       </c>
@@ -4603,7 +4617,7 @@
         <v>31</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="D99" s="30"/>
       <c r="E99" s="30" t="s">
@@ -4613,10 +4627,10 @@
         <v>6</v>
       </c>
       <c r="G99" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H99" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I99" s="32"/>
     </row>
@@ -4628,7 +4642,7 @@
         <v>31</v>
       </c>
       <c r="C100" s="32" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="D100" s="30"/>
       <c r="E100" s="30" t="s">
@@ -4652,8 +4666,8 @@
       <c r="B101" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C101" s="32" t="s">
-        <v>246</v>
+      <c r="C101" s="20" t="s">
+        <v>232</v>
       </c>
       <c r="D101" s="30"/>
       <c r="E101" s="30" t="s">
@@ -4670,7 +4684,7 @@
       </c>
       <c r="I101" s="32"/>
     </row>
-    <row r="102" spans="1:9" ht="30">
+    <row r="102" spans="1:9" ht="45">
       <c r="A102" s="30" t="s">
         <v>124</v>
       </c>
@@ -4678,24 +4692,24 @@
         <v>31</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F102" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G102" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H102" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I102" s="32"/>
     </row>
-    <row r="103" spans="1:9" ht="45">
+    <row r="103" spans="1:9" ht="180">
       <c r="A103" s="30" t="s">
         <v>125</v>
       </c>
@@ -4703,7 +4717,7 @@
         <v>31</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="D103" s="30"/>
       <c r="E103" s="30" t="s">
@@ -4720,7 +4734,7 @@
       </c>
       <c r="I103" s="32"/>
     </row>
-    <row r="104" spans="1:9" ht="180">
+    <row r="104" spans="1:9" ht="30">
       <c r="A104" s="30" t="s">
         <v>126</v>
       </c>
@@ -4728,24 +4742,24 @@
         <v>31</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="D104" s="30"/>
       <c r="E104" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F104" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G104" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H104" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9">
       <c r="A105" s="30" t="s">
         <v>127</v>
       </c>
@@ -4753,7 +4767,7 @@
         <v>31</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="D105" s="30"/>
       <c r="E105" s="30" t="s">
@@ -4763,22 +4777,22 @@
         <v>6</v>
       </c>
       <c r="G105" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H105" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" ht="30">
       <c r="A106" s="30" t="s">
         <v>128</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="D106" s="30"/>
       <c r="E106" s="30" t="s">
@@ -4788,10 +4802,10 @@
         <v>6</v>
       </c>
       <c r="G106" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H106" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I106" s="32"/>
     </row>
@@ -4803,7 +4817,7 @@
         <v>32</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="D107" s="30"/>
       <c r="E107" s="30" t="s">
@@ -4828,7 +4842,7 @@
         <v>32</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="D108" s="30"/>
       <c r="E108" s="30" t="s">
@@ -4845,7 +4859,7 @@
       </c>
       <c r="I108" s="32"/>
     </row>
-    <row r="109" spans="1:9" ht="45">
+    <row r="109" spans="1:9" ht="30">
       <c r="A109" s="30" t="s">
         <v>131</v>
       </c>
@@ -4853,7 +4867,7 @@
         <v>32</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="D109" s="30"/>
       <c r="E109" s="30" t="s">
@@ -4877,8 +4891,8 @@
       <c r="B110" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C110" s="32" t="s">
-        <v>255</v>
+      <c r="C110" s="20" t="s">
+        <v>276</v>
       </c>
       <c r="D110" s="30"/>
       <c r="E110" s="30" t="s">
@@ -4903,7 +4917,7 @@
         <v>32</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="D111" s="30"/>
       <c r="E111" s="30" t="s">
@@ -4920,7 +4934,7 @@
       </c>
       <c r="I111" s="32"/>
     </row>
-    <row r="112" spans="1:9" ht="45">
+    <row r="112" spans="1:9" ht="30">
       <c r="A112" s="30" t="s">
         <v>134</v>
       </c>
@@ -4928,7 +4942,7 @@
         <v>32</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="D112" s="30"/>
       <c r="E112" s="30" t="s">
@@ -4941,11 +4955,11 @@
         <v>15</v>
       </c>
       <c r="H112" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="45">
+    <row r="113" spans="1:9" ht="30">
       <c r="A113" s="30" t="s">
         <v>135</v>
       </c>
@@ -4953,7 +4967,7 @@
         <v>32</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="D113" s="30"/>
       <c r="E113" s="30" t="s">
@@ -4970,7 +4984,7 @@
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9" ht="45">
+    <row r="114" spans="1:9">
       <c r="A114" s="30" t="s">
         <v>136</v>
       </c>
@@ -4978,7 +4992,7 @@
         <v>32</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30" t="s">
@@ -4988,22 +5002,22 @@
         <v>6</v>
       </c>
       <c r="G114" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H114" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I114" s="32"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" ht="30">
       <c r="A115" s="30" t="s">
         <v>137</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>32</v>
+        <v>161</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="D115" s="30"/>
       <c r="E115" s="30" t="s">
@@ -5013,10 +5027,10 @@
         <v>6</v>
       </c>
       <c r="G115" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H115" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I115" s="32"/>
     </row>
@@ -5025,35 +5039,35 @@
         <v>138</v>
       </c>
       <c r="B116" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F116" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G116" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H116" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I116" s="32"/>
     </row>
-    <row r="117" spans="1:9" ht="45">
+    <row r="117" spans="1:9" ht="30">
       <c r="A117" s="30" t="s">
         <v>139</v>
       </c>
       <c r="B117" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="D117" s="30"/>
       <c r="E117" s="30" t="s">
@@ -5070,15 +5084,15 @@
       </c>
       <c r="I117" s="32"/>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9">
       <c r="A118" s="30" t="s">
         <v>140</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="D118" s="30"/>
       <c r="E118" s="30" t="s">
@@ -5095,90 +5109,90 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" ht="30">
       <c r="A119" s="30" t="s">
         <v>141</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="D119" s="30"/>
       <c r="E119" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F119" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G119" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H119" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I119" s="32"/>
     </row>
-    <row r="120" spans="1:9" ht="30">
+    <row r="120" spans="1:9" ht="270">
       <c r="A120" s="30" t="s">
         <v>142</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="D120" s="30"/>
       <c r="E120" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F120" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G120" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H120" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9" ht="270">
+    <row r="121" spans="1:9" ht="30">
       <c r="A121" s="30" t="s">
         <v>143</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="D121" s="30"/>
       <c r="E121" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F121" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G121" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H121" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I121" s="32"/>
     </row>
-    <row r="122" spans="1:9" ht="30">
+    <row r="122" spans="1:9">
       <c r="A122" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="D122" s="30"/>
       <c r="E122" s="30" t="s">
@@ -5188,29 +5202,29 @@
         <v>6</v>
       </c>
       <c r="G122" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H122" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" ht="45">
       <c r="A123" s="30" t="s">
         <v>145</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="D123" s="30"/>
       <c r="E123" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F123" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G123" s="30" t="s">
         <v>16</v>
@@ -5220,15 +5234,15 @@
       </c>
       <c r="I123" s="32"/>
     </row>
-    <row r="124" spans="1:9" ht="45">
+    <row r="124" spans="1:9" ht="30">
       <c r="A124" s="30" t="s">
         <v>146</v>
       </c>
       <c r="B124" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="D124" s="30"/>
       <c r="E124" s="30" t="s">
@@ -5245,99 +5259,50 @@
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" ht="30">
+    <row r="125" spans="1:9" ht="45">
       <c r="A125" s="30" t="s">
         <v>147</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C125" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="D125" s="30"/>
+        <v>251</v>
+      </c>
+      <c r="D125" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="E125" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F125" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G125" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H125" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I125" s="32"/>
-    </row>
-    <row r="126" spans="1:9" ht="45">
-      <c r="A126" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="B126" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="C126" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="D126" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="E126" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F126" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="G126" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H126" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I126" s="32" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" ht="45">
-      <c r="A127" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="B127" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="C127" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="D127" s="30" t="s">
-        <v>276</v>
-      </c>
-      <c r="E127" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F127" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="G127" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H127" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I127" s="32" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
-      <c r="A128" s="3"/>
-      <c r="B128" s="10"/>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="3"/>
-      <c r="B129" s="10"/>
+      <c r="I125" s="32" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" s="3"/>
+      <c r="B126" s="10"/>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" s="3"/>
+      <c r="B127" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -5345,14 +5310,9 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I20:I127 A20:H125 A34:I127">
+  <conditionalFormatting sqref="A33:I125 A22:H124 I22:I125 A20:I21">
     <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -5363,7 +5323,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I127 A20:H125 A34:I127">
+  <conditionalFormatting sqref="A33:I125 A22:H124 I22:I125 A20:I21">
     <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -5374,7 +5334,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F127">
+  <conditionalFormatting sqref="F20:F125">
     <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -5383,20 +5343,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F127">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F125">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E127">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E125">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G127">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G125">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H127">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H125">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5406,7 +5366,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B19:B125 B126:B129 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B19 B125 B126:B127 B21:B124 B20 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -5416,6 +5376,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -5464,12 +5430,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5480,6 +5440,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5494,20 +5468,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[MS-WSSREST]: Add new cases and capture code for 3 fixed TDIs\TDQs
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WSSREST/MS-WSSREST_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WSSREST/MS-WSSREST_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -1362,6 +1362,21 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1385,21 +1400,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2342,127 +2342,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -2475,12 +2475,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -2493,12 +2493,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -2511,12 +2511,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -2529,60 +2529,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -3514,7 +3514,7 @@
         <v>15</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I55" s="32"/>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="30">
+    <row r="67" spans="1:9">
       <c r="A67" s="30" t="s">
         <v>89</v>
       </c>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9" ht="30">
+    <row r="121" spans="1:9">
       <c r="A121" s="30" t="s">
         <v>143</v>
       </c>
@@ -5298,11 +5298,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -5310,6 +5305,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A33:I125 A22:H124 I22:I125 A20:I21">
@@ -5376,9 +5376,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5431,24 +5434,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5469,9 +5463,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>